<commit_message>
termino entregable sprint 1
</commit_message>
<xml_diff>
--- a/Documentacion/Product Backlog/Product Backlog.xlsx
+++ b/Documentacion/Product Backlog/Product Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victoria\Desktop\UTP\programacion\ciclo4_Desarrollo_Web\Proyecto\Documentacion\Product Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3057C355-F141-40D7-B0E3-FBD9AE3980EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94BEC6B-5016-4D23-85CE-5EAB974C825F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="2160" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Release Plan" sheetId="1" r:id="rId1"/>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="76">
   <si>
     <t>Increment Plan</t>
   </si>
@@ -6692,7 +6692,7 @@
   <dimension ref="A1:Z992"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6982,7 +6982,7 @@
     </row>
     <row r="8" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" s="25" t="s">
         <v>22</v>
@@ -7024,7 +7024,7 @@
     </row>
     <row r="9" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="25" t="s">
         <v>45</v>
@@ -7132,7 +7132,7 @@
       </c>
       <c r="D12" s="27"/>
       <c r="E12" s="25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" s="25">
         <v>1</v>
@@ -7172,7 +7172,7 @@
       </c>
       <c r="D13" s="27"/>
       <c r="E13" s="25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" s="25">
         <v>1</v>

</xml_diff>